<commit_message>
add delete account feature
</commit_message>
<xml_diff>
--- a/resources/DataPurchase.xlsx
+++ b/resources/DataPurchase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/G2Lab/FinalProject/QuotaAppTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E10F167-7E5D-6543-AC3E-39573A8E6E38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D00E1E-F642-DE42-BE3D-0073DCEB04AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{57623300-8E2D-C54C-A558-4EEA7A09C665}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1290" uniqueCount="119">
   <si>
     <t>description</t>
   </si>
@@ -94,30 +94,6 @@
     <t>Mentari</t>
   </si>
   <si>
-    <t>+6281absurdomor</t>
-  </si>
-  <si>
-    <t>negative case - invalid phone number (blank)</t>
-  </si>
-  <si>
-    <t>negative case - invalid phone number (not numerical only)</t>
-  </si>
-  <si>
-    <t>+628125293039X</t>
-  </si>
-  <si>
-    <t>+6281252C30398</t>
-  </si>
-  <si>
-    <t>081252930xyz</t>
-  </si>
-  <si>
-    <t>0812529M5671</t>
-  </si>
-  <si>
-    <t>notnumericalonly</t>
-  </si>
-  <si>
     <t>+6281235671985</t>
   </si>
   <si>
@@ -172,12 +148,6 @@
     <t>responseBodyInvoice</t>
   </si>
   <si>
-    <t>404</t>
-  </si>
-  <si>
-    <t>Not Found</t>
-  </si>
-  <si>
     <t>negative case - invalid phone number, phone number for paket data, provider, price, paket data</t>
   </si>
   <si>
@@ -362,6 +332,66 @@
   </si>
   <si>
     <t>DANA.jpg</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number, pin transaction</t>
+  </si>
+  <si>
+    <t>negative case - invalid pin transaction</t>
+  </si>
+  <si>
+    <t>positive case - valid phone number, pin transaction</t>
+  </si>
+  <si>
+    <t>negative case - invalid pin transaction (below 6 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid pin transaction (exceed 6 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid pin transaction (not numerical only)</t>
+  </si>
+  <si>
+    <t>negative case - invalid virtual account (not numerical only)</t>
+  </si>
+  <si>
+    <t>negative case - invalid virtual account (exceed 19 characters)</t>
+  </si>
+  <si>
+    <t>negative case - invalid phone number, virtual account</t>
+  </si>
+  <si>
+    <t>negative case - invalid virtual account</t>
+  </si>
+  <si>
+    <t>positive case - valid phone number, virtual account</t>
+  </si>
+  <si>
+    <t>not numerical only</t>
+  </si>
+  <si>
+    <t>800008125293039812345678</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>inipin</t>
+  </si>
+  <si>
+    <t>+6285851791667</t>
+  </si>
+  <si>
+    <t>+6285705917901</t>
+  </si>
+  <si>
+    <t>+6285765345721</t>
+  </si>
+  <si>
+    <t>+6281261351971</t>
   </si>
 </sst>
 </file>
@@ -449,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -471,6 +501,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -793,12 +827,12 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B18" sqref="B18:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -904,11 +938,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
+      <c r="A8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>10</v>
@@ -918,11 +952,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
+      <c r="A9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>10</v>
@@ -932,11 +966,11 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>23</v>
+      <c r="A10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>10</v>
@@ -946,11 +980,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>24</v>
+      <c r="A11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>10</v>
@@ -960,11 +994,11 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>25</v>
+      <c r="A12" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>10</v>
@@ -974,53 +1008,59 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>11</v>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>11</v>
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1028,13 +1068,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,7 +1082,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>8</v>
@@ -1056,13 +1096,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1070,13 +1110,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1084,13 +1124,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1101,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8D8A7E-F8A4-4F41-BE15-873B0010E036}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1160,7 @@
     <col min="9" max="9" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="49.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -1137,16 +1177,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1155,36 +1195,36 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>7</v>
@@ -1193,51 +1233,51 @@
         <v>7</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>7</v>
@@ -1246,51 +1286,51 @@
         <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>7</v>
@@ -1299,51 +1339,51 @@
         <v>7</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>7</v>
@@ -1352,51 +1392,51 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>7</v>
@@ -1411,45 +1451,45 @@
         <v>7</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>7</v>
@@ -1464,45 +1504,45 @@
         <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>7</v>
@@ -1514,48 +1554,48 @@
         <v>9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>7</v>
@@ -1567,48 +1607,48 @@
         <v>9</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>7</v>
@@ -1617,51 +1657,51 @@
         <v>6</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>7</v>
@@ -1670,51 +1710,51 @@
         <v>6</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>7</v>
@@ -1723,51 +1763,51 @@
         <v>6</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>7</v>
@@ -1776,51 +1816,51 @@
         <v>6</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>7</v>
@@ -1835,45 +1875,45 @@
         <v>7</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>7</v>
@@ -1888,45 +1928,45 @@
         <v>7</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>7</v>
@@ -1938,43 +1978,43 @@
         <v>9</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -1991,48 +2031,48 @@
         <v>9</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>6</v>
@@ -2041,104 +2081,104 @@
         <v>7</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="I19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>6</v>
@@ -2147,51 +2187,51 @@
         <v>7</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>6</v>
@@ -2200,51 +2240,51 @@
         <v>7</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>6</v>
@@ -2259,45 +2299,45 @@
         <v>7</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>6</v>
@@ -2312,45 +2352,45 @@
         <v>7</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>6</v>
@@ -2362,48 +2402,48 @@
         <v>9</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>6</v>
@@ -2415,48 +2455,48 @@
         <v>9</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>6</v>
@@ -2465,51 +2505,51 @@
         <v>6</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>6</v>
@@ -2518,51 +2558,51 @@
         <v>6</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>6</v>
@@ -2571,51 +2611,51 @@
         <v>6</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>6</v>
@@ -2624,13 +2664,13 @@
         <v>6</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>10</v>
@@ -2639,36 +2679,36 @@
         <v>10</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>6</v>
@@ -2683,45 +2723,45 @@
         <v>7</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>6</v>
@@ -2736,45 +2776,45 @@
         <v>7</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>6</v>
@@ -2786,10 +2826,10 @@
         <v>9</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>10</v>
@@ -2798,36 +2838,36 @@
         <v>10</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>6</v>
@@ -2839,51 +2879,51 @@
         <v>9</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>8</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>6</v>
+      <c r="A34" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>6</v>
@@ -2892,51 +2932,51 @@
         <v>9</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="P34" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q34" s="4" t="s">
-        <v>8</v>
+        <v>69</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q34" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>7</v>
+        <v>75</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>6</v>
@@ -2945,51 +2985,51 @@
         <v>9</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>6</v>
@@ -2998,51 +3038,51 @@
         <v>9</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>6</v>
@@ -3051,51 +3091,51 @@
         <v>9</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>6</v>
@@ -3104,366 +3144,366 @@
         <v>9</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>6</v>
+        <v>79</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>7</v>
+      <c r="C40" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>9</v>
+      <c r="C44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>6</v>
@@ -3471,153 +3511,1311 @@
       <c r="C45" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>80</v>
+      <c r="D45" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>10</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="O45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="P45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q45" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P46" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q47" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J48" s="3"/>
+      <c r="K48" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I49" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N50" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I46" s="3" t="s">
+      <c r="O50" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="P50" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J51" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P51" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I53" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M53" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N53" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q53" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J54" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P54" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P55" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q55" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="J46" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M46" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="N46" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O46" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="P46" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q46" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
+      <c r="B56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M56" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q56" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I57" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I58" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K58" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N58" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L60" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="L47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="N47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="O47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="P47" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q47" s="3" t="s">
-        <v>102</v>
+      <c r="M60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N60" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O60" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P60" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q60" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K61" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L61" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N61" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O61" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P61" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q61" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K62" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N62" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="O62" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="P62" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q62" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A63" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N63" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O63" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P63" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q63" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A64" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I64" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J64" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L64" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O64" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P64" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A65" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I65" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J65" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L65" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N65" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O65" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P65" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q65" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A66" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I66" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J66" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L66" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O66" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P66" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q66" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A67" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I67" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J67" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L67" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O67" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P67" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q67" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I68" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L68" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O68" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P68" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I69" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L69" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="P69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q69" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3630,7 +4828,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3680,11 +4878,11 @@
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
+      <c r="A4" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>8</v>
@@ -3692,11 +4890,11 @@
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>22</v>
+      <c r="A5" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>8</v>
@@ -3704,11 +4902,11 @@
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
+      <c r="A6" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
@@ -3716,11 +4914,11 @@
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>24</v>
+      <c r="A7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>8</v>
@@ -3728,11 +4926,11 @@
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>25</v>
+      <c r="A8" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>8</v>
@@ -3740,52 +4938,52 @@
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6"/>
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>46</v>
-      </c>
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>